<commit_message>
se en list v exelu
</commit_message>
<xml_diff>
--- a/rezultati_naloga_2.xlsx
+++ b/rezultati_naloga_2.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="dimenzija za m=4" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="dimenzija za m=5-10" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -720,4 +721,850 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Ni definirano za m &gt;= n</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Ni definirano za m &gt;= n</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Ni definirano za m &gt;= n</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Ni definirano za m &gt;= n</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Ni definirano za m &gt;= n</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Ni definirano za m &gt;= n</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ni definirano za m &gt;= n</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Ni definirano za m &gt;= n</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ni definirano za m &gt;= n</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ni definirano za m &gt;= n</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B9" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" t="n">
+        <v>5</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B11" t="n">
+        <v>7</v>
+      </c>
+      <c r="C11" t="n">
+        <v>7</v>
+      </c>
+      <c r="D11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8</v>
+      </c>
+      <c r="F11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B12" t="n">
+        <v>7</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7</v>
+      </c>
+      <c r="D12" t="n">
+        <v>7</v>
+      </c>
+      <c r="E12" t="n">
+        <v>7</v>
+      </c>
+      <c r="F12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B13" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>7</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>9</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B14" t="n">
+        <v>8</v>
+      </c>
+      <c r="C14" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" t="n">
+        <v>8</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" t="n">
+        <v>8</v>
+      </c>
+      <c r="G14" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B15" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>8</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8</v>
+      </c>
+      <c r="G15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B16" t="n">
+        <v>7</v>
+      </c>
+      <c r="C16" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" t="n">
+        <v>8</v>
+      </c>
+      <c r="E16" t="n">
+        <v>7</v>
+      </c>
+      <c r="F16" t="n">
+        <v>9</v>
+      </c>
+      <c r="G16" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B17" t="n">
+        <v>9</v>
+      </c>
+      <c r="C17" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" t="n">
+        <v>9</v>
+      </c>
+      <c r="E17" t="n">
+        <v>9</v>
+      </c>
+      <c r="F17" t="n">
+        <v>9</v>
+      </c>
+      <c r="G17" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B18" t="n">
+        <v>9</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10</v>
+      </c>
+      <c r="D18" t="n">
+        <v>9</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B19" t="n">
+        <v>8</v>
+      </c>
+      <c r="C19" t="n">
+        <v>10</v>
+      </c>
+      <c r="D19" t="n">
+        <v>9</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+      <c r="F19" t="n">
+        <v>9</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B20" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" t="n">
+        <v>10</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10</v>
+      </c>
+      <c r="G20" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B21" t="n">
+        <v>10</v>
+      </c>
+      <c r="C21" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
+        <v>11</v>
+      </c>
+      <c r="F21" t="n">
+        <v>11</v>
+      </c>
+      <c r="G21" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B22" t="n">
+        <v>9</v>
+      </c>
+      <c r="C22" t="n">
+        <v>11</v>
+      </c>
+      <c r="D22" t="n">
+        <v>11</v>
+      </c>
+      <c r="E22" t="n">
+        <v>9</v>
+      </c>
+      <c r="F22" t="n">
+        <v>10</v>
+      </c>
+      <c r="G22" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B23" t="n">
+        <v>11</v>
+      </c>
+      <c r="C23" t="n">
+        <v>11</v>
+      </c>
+      <c r="D23" t="n">
+        <v>11</v>
+      </c>
+      <c r="E23" t="n">
+        <v>11</v>
+      </c>
+      <c r="F23" t="n">
+        <v>12</v>
+      </c>
+      <c r="G23" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B24" t="n">
+        <v>11</v>
+      </c>
+      <c r="C24" t="n">
+        <v>11</v>
+      </c>
+      <c r="D24" t="n">
+        <v>11</v>
+      </c>
+      <c r="E24" t="n">
+        <v>12</v>
+      </c>
+      <c r="F24" t="n">
+        <v>12</v>
+      </c>
+      <c r="G24" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B25" t="n">
+        <v>10</v>
+      </c>
+      <c r="C25" t="n">
+        <v>12</v>
+      </c>
+      <c r="D25" t="n">
+        <v>12</v>
+      </c>
+      <c r="E25" t="n">
+        <v>10</v>
+      </c>
+      <c r="F25" t="n">
+        <v>12</v>
+      </c>
+      <c r="G25" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B26" t="n">
+        <v>12</v>
+      </c>
+      <c r="C26" t="n">
+        <v>12</v>
+      </c>
+      <c r="D26" t="n">
+        <v>12</v>
+      </c>
+      <c r="E26" t="n">
+        <v>13</v>
+      </c>
+      <c r="F26" t="n">
+        <v>12</v>
+      </c>
+      <c r="G26" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B27" t="n">
+        <v>12</v>
+      </c>
+      <c r="C27" t="n">
+        <v>13</v>
+      </c>
+      <c r="D27" t="n">
+        <v>12</v>
+      </c>
+      <c r="E27" t="n">
+        <v>13</v>
+      </c>
+      <c r="F27" t="n">
+        <v>13</v>
+      </c>
+      <c r="G27" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B28" t="n">
+        <v>11</v>
+      </c>
+      <c r="C28" t="n">
+        <v>12</v>
+      </c>
+      <c r="D28" t="n">
+        <v>13</v>
+      </c>
+      <c r="E28" t="n">
+        <v>11</v>
+      </c>
+      <c r="F28" t="n">
+        <v>14</v>
+      </c>
+      <c r="G28" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B29" t="n">
+        <v>13</v>
+      </c>
+      <c r="C29" t="n">
+        <v>14</v>
+      </c>
+      <c r="D29" t="n">
+        <v>13</v>
+      </c>
+      <c r="E29" t="n">
+        <v>14</v>
+      </c>
+      <c r="F29" t="n">
+        <v>12</v>
+      </c>
+      <c r="G29" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B30" t="n">
+        <v>13</v>
+      </c>
+      <c r="C30" t="n">
+        <v>14</v>
+      </c>
+      <c r="D30" t="n">
+        <v>14</v>
+      </c>
+      <c r="E30" t="n">
+        <v>14</v>
+      </c>
+      <c r="F30" t="n">
+        <v>14</v>
+      </c>
+      <c r="G30" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B31" t="n">
+        <v>12</v>
+      </c>
+      <c r="C31" t="n">
+        <v>14</v>
+      </c>
+      <c r="D31" t="n">
+        <v>14</v>
+      </c>
+      <c r="E31" t="n">
+        <v>12</v>
+      </c>
+      <c r="F31" t="n">
+        <v>14</v>
+      </c>
+      <c r="G31" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B32" t="n">
+        <v>14</v>
+      </c>
+      <c r="C32" t="n">
+        <v>14</v>
+      </c>
+      <c r="D32" t="n">
+        <v>14</v>
+      </c>
+      <c r="E32" t="n">
+        <v>15</v>
+      </c>
+      <c r="F32" t="n">
+        <v>14</v>
+      </c>
+      <c r="G32" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B33" t="n">
+        <v>14</v>
+      </c>
+      <c r="C33" t="n">
+        <v>15</v>
+      </c>
+      <c r="D33" t="n">
+        <v>15</v>
+      </c>
+      <c r="E33" t="n">
+        <v>15</v>
+      </c>
+      <c r="F33" t="n">
+        <v>15</v>
+      </c>
+      <c r="G33" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B34" t="n">
+        <v>13</v>
+      </c>
+      <c r="C34" t="n">
+        <v>15</v>
+      </c>
+      <c r="D34" t="n">
+        <v>15</v>
+      </c>
+      <c r="E34" t="n">
+        <v>13</v>
+      </c>
+      <c r="F34" t="n">
+        <v>15</v>
+      </c>
+      <c r="G34" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B35" t="n">
+        <v>15</v>
+      </c>
+      <c r="C35" t="n">
+        <v>15</v>
+      </c>
+      <c r="D35" t="n">
+        <v>15</v>
+      </c>
+      <c r="E35" t="n">
+        <v>16</v>
+      </c>
+      <c r="F35" t="n">
+        <v>16</v>
+      </c>
+      <c r="G35" t="n">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
rezultati za n od 7 do 40
</commit_message>
<xml_diff>
--- a/rezultati_naloga_2.xlsx
+++ b/rezultati_naloga_2.xlsx
@@ -440,10 +440,8 @@
           <t>n</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="2">
@@ -772,26 +770,10 @@
       <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Ni definirano za m &gt;= n</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Ni definirano za m &gt;= n</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Ni definirano za m &gt;= n</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Ni definirano za m &gt;= n</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -806,21 +788,9 @@
       <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Ni definirano za m &gt;= n</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Ni definirano za m &gt;= n</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Ni definirano za m &gt;= n</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -838,16 +808,8 @@
       <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Ni definirano za m &gt;= n</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Ni definirano za m &gt;= n</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -868,11 +830,7 @@
       <c r="F5" t="n">
         <v>1</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Ni definirano za m &gt;= n</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">

</xml_diff>

<commit_message>
rezultati za n od 7 do 77
</commit_message>
<xml_diff>
--- a/rezultati_naloga_2.xlsx
+++ b/rezultati_naloga_2.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,6 +716,302 @@
         <v>16</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B36" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B37" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B38" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B39" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B40" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B41" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B42" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B43" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B44" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B45" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B46" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B47" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B48" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B49" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B50" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B51" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B52" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B53" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B54" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B55" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B56" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B57" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B58" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B59" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B60" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B61" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B62" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B63" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B64" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B65" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B66" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B67" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B68" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B69" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B70" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B71" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B72" t="n">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -727,7 +1023,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1522,6 +1818,857 @@
         <v>15</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B36" t="n">
+        <v>15</v>
+      </c>
+      <c r="C36" t="n">
+        <v>16</v>
+      </c>
+      <c r="D36" t="n">
+        <v>16</v>
+      </c>
+      <c r="E36" t="n">
+        <v>16</v>
+      </c>
+      <c r="F36" t="n">
+        <v>15</v>
+      </c>
+      <c r="G36" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B37" t="n">
+        <v>14</v>
+      </c>
+      <c r="C37" t="n">
+        <v>16</v>
+      </c>
+      <c r="D37" t="n">
+        <v>16</v>
+      </c>
+      <c r="E37" t="n">
+        <v>14</v>
+      </c>
+      <c r="F37" t="n">
+        <v>17</v>
+      </c>
+      <c r="G37" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B38" t="n">
+        <v>16</v>
+      </c>
+      <c r="C38" t="n">
+        <v>17</v>
+      </c>
+      <c r="D38" t="n">
+        <v>17</v>
+      </c>
+      <c r="E38" t="n">
+        <v>17</v>
+      </c>
+      <c r="F38" t="n">
+        <v>17</v>
+      </c>
+      <c r="G38" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B39" t="n">
+        <v>16</v>
+      </c>
+      <c r="C39" t="n">
+        <v>16</v>
+      </c>
+      <c r="D39" t="n">
+        <v>17</v>
+      </c>
+      <c r="E39" t="n">
+        <v>17</v>
+      </c>
+      <c r="F39" t="n">
+        <v>16</v>
+      </c>
+      <c r="G39" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B40" t="n">
+        <v>15</v>
+      </c>
+      <c r="C40" t="n">
+        <v>18</v>
+      </c>
+      <c r="D40" t="n">
+        <v>17</v>
+      </c>
+      <c r="E40" t="n">
+        <v>15</v>
+      </c>
+      <c r="F40" t="n">
+        <v>18</v>
+      </c>
+      <c r="G40" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B41" t="n">
+        <v>17</v>
+      </c>
+      <c r="C41" t="n">
+        <v>18</v>
+      </c>
+      <c r="D41" t="n">
+        <v>18</v>
+      </c>
+      <c r="E41" t="n">
+        <v>18</v>
+      </c>
+      <c r="F41" t="n">
+        <v>18</v>
+      </c>
+      <c r="G41" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B42" t="n">
+        <v>17</v>
+      </c>
+      <c r="C42" t="n">
+        <v>18</v>
+      </c>
+      <c r="D42" t="n">
+        <v>18</v>
+      </c>
+      <c r="E42" t="n">
+        <v>18</v>
+      </c>
+      <c r="F42" t="n">
+        <v>18</v>
+      </c>
+      <c r="G42" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B43" t="n">
+        <v>16</v>
+      </c>
+      <c r="C43" t="n">
+        <v>18</v>
+      </c>
+      <c r="D43" t="n">
+        <v>18</v>
+      </c>
+      <c r="E43" t="n">
+        <v>16</v>
+      </c>
+      <c r="F43" t="n">
+        <v>18</v>
+      </c>
+      <c r="G43" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B44" t="n">
+        <v>18</v>
+      </c>
+      <c r="C44" t="n">
+        <v>19</v>
+      </c>
+      <c r="D44" t="n">
+        <v>19</v>
+      </c>
+      <c r="E44" t="n">
+        <v>19</v>
+      </c>
+      <c r="F44" t="n">
+        <v>19</v>
+      </c>
+      <c r="G44" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B45" t="n">
+        <v>18</v>
+      </c>
+      <c r="C45" t="n">
+        <v>19</v>
+      </c>
+      <c r="D45" t="n">
+        <v>19</v>
+      </c>
+      <c r="E45" t="n">
+        <v>19</v>
+      </c>
+      <c r="F45" t="n">
+        <v>20</v>
+      </c>
+      <c r="G45" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B46" t="n">
+        <v>17</v>
+      </c>
+      <c r="C46" t="n">
+        <v>19</v>
+      </c>
+      <c r="D46" t="n">
+        <v>20</v>
+      </c>
+      <c r="E46" t="n">
+        <v>17</v>
+      </c>
+      <c r="F46" t="n">
+        <v>18</v>
+      </c>
+      <c r="G46" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B47" t="n">
+        <v>19</v>
+      </c>
+      <c r="C47" t="n">
+        <v>20</v>
+      </c>
+      <c r="D47" t="n">
+        <v>20</v>
+      </c>
+      <c r="E47" t="n">
+        <v>20</v>
+      </c>
+      <c r="F47" t="n">
+        <v>21</v>
+      </c>
+      <c r="G47" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B48" t="n">
+        <v>19</v>
+      </c>
+      <c r="C48" t="n">
+        <v>20</v>
+      </c>
+      <c r="D48" t="n">
+        <v>20</v>
+      </c>
+      <c r="E48" t="n">
+        <v>20</v>
+      </c>
+      <c r="F48" t="n">
+        <v>20</v>
+      </c>
+      <c r="G48" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B49" t="n">
+        <v>18</v>
+      </c>
+      <c r="C49" t="n">
+        <v>21</v>
+      </c>
+      <c r="D49" t="n">
+        <v>21</v>
+      </c>
+      <c r="E49" t="n">
+        <v>18</v>
+      </c>
+      <c r="F49" t="n">
+        <v>20</v>
+      </c>
+      <c r="G49" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B50" t="n">
+        <v>20</v>
+      </c>
+      <c r="C50" t="n">
+        <v>20</v>
+      </c>
+      <c r="D50" t="n">
+        <v>21</v>
+      </c>
+      <c r="E50" t="n">
+        <v>21</v>
+      </c>
+      <c r="F50" t="n">
+        <v>21</v>
+      </c>
+      <c r="G50" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B51" t="n">
+        <v>20</v>
+      </c>
+      <c r="C51" t="n">
+        <v>22</v>
+      </c>
+      <c r="D51" t="n">
+        <v>21</v>
+      </c>
+      <c r="E51" t="n">
+        <v>21</v>
+      </c>
+      <c r="F51" t="n">
+        <v>21</v>
+      </c>
+      <c r="G51" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B52" t="n">
+        <v>19</v>
+      </c>
+      <c r="C52" t="n">
+        <v>22</v>
+      </c>
+      <c r="D52" t="n">
+        <v>22</v>
+      </c>
+      <c r="E52" t="n">
+        <v>19</v>
+      </c>
+      <c r="F52" t="n">
+        <v>22</v>
+      </c>
+      <c r="G52" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B53" t="n">
+        <v>21</v>
+      </c>
+      <c r="C53" t="n">
+        <v>22</v>
+      </c>
+      <c r="D53" t="n">
+        <v>22</v>
+      </c>
+      <c r="E53" t="n">
+        <v>22</v>
+      </c>
+      <c r="F53" t="n">
+        <v>21</v>
+      </c>
+      <c r="G53" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B54" t="n">
+        <v>21</v>
+      </c>
+      <c r="C54" t="n">
+        <v>22</v>
+      </c>
+      <c r="D54" t="n">
+        <v>23</v>
+      </c>
+      <c r="E54" t="n">
+        <v>22</v>
+      </c>
+      <c r="F54" t="n">
+        <v>23</v>
+      </c>
+      <c r="G54" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B55" t="n">
+        <v>20</v>
+      </c>
+      <c r="C55" t="n">
+        <v>23</v>
+      </c>
+      <c r="D55" t="n">
+        <v>23</v>
+      </c>
+      <c r="E55" t="n">
+        <v>20</v>
+      </c>
+      <c r="F55" t="n">
+        <v>23</v>
+      </c>
+      <c r="G55" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B56" t="n">
+        <v>22</v>
+      </c>
+      <c r="C56" t="n">
+        <v>23</v>
+      </c>
+      <c r="D56" t="n">
+        <v>23</v>
+      </c>
+      <c r="E56" t="n">
+        <v>23</v>
+      </c>
+      <c r="F56" t="n">
+        <v>22</v>
+      </c>
+      <c r="G56" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B57" t="n">
+        <v>22</v>
+      </c>
+      <c r="C57" t="n">
+        <v>23</v>
+      </c>
+      <c r="D57" t="n">
+        <v>24</v>
+      </c>
+      <c r="E57" t="n">
+        <v>23</v>
+      </c>
+      <c r="F57" t="n">
+        <v>24</v>
+      </c>
+      <c r="G57" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B58" t="n">
+        <v>21</v>
+      </c>
+      <c r="C58" t="n">
+        <v>24</v>
+      </c>
+      <c r="D58" t="n">
+        <v>24</v>
+      </c>
+      <c r="E58" t="n">
+        <v>21</v>
+      </c>
+      <c r="F58" t="n">
+        <v>24</v>
+      </c>
+      <c r="G58" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B59" t="n">
+        <v>23</v>
+      </c>
+      <c r="C59" t="n">
+        <v>24</v>
+      </c>
+      <c r="D59" t="n">
+        <v>24</v>
+      </c>
+      <c r="E59" t="n">
+        <v>24</v>
+      </c>
+      <c r="F59" t="n">
+        <v>24</v>
+      </c>
+      <c r="G59" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B60" t="n">
+        <v>23</v>
+      </c>
+      <c r="C60" t="n">
+        <v>25</v>
+      </c>
+      <c r="D60" t="n">
+        <v>25</v>
+      </c>
+      <c r="E60" t="n">
+        <v>24</v>
+      </c>
+      <c r="F60" t="n">
+        <v>24</v>
+      </c>
+      <c r="G60" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B61" t="n">
+        <v>22</v>
+      </c>
+      <c r="C61" t="n">
+        <v>24</v>
+      </c>
+      <c r="D61" t="n">
+        <v>25</v>
+      </c>
+      <c r="E61" t="n">
+        <v>22</v>
+      </c>
+      <c r="F61" t="n">
+        <v>25</v>
+      </c>
+      <c r="G61" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B62" t="n">
+        <v>24</v>
+      </c>
+      <c r="C62" t="n">
+        <v>26</v>
+      </c>
+      <c r="D62" t="n">
+        <v>26</v>
+      </c>
+      <c r="E62" t="n">
+        <v>25</v>
+      </c>
+      <c r="F62" t="n">
+        <v>26</v>
+      </c>
+      <c r="G62" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B63" t="n">
+        <v>24</v>
+      </c>
+      <c r="C63" t="n">
+        <v>26</v>
+      </c>
+      <c r="D63" t="n">
+        <v>26</v>
+      </c>
+      <c r="E63" t="n">
+        <v>25</v>
+      </c>
+      <c r="F63" t="n">
+        <v>24</v>
+      </c>
+      <c r="G63" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B64" t="n">
+        <v>23</v>
+      </c>
+      <c r="C64" t="n">
+        <v>26</v>
+      </c>
+      <c r="D64" t="n">
+        <v>26</v>
+      </c>
+      <c r="E64" t="n">
+        <v>23</v>
+      </c>
+      <c r="F64" t="n">
+        <v>27</v>
+      </c>
+      <c r="G64" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B65" t="n">
+        <v>25</v>
+      </c>
+      <c r="C65" t="n">
+        <v>26</v>
+      </c>
+      <c r="D65" t="n">
+        <v>27</v>
+      </c>
+      <c r="E65" t="n">
+        <v>26</v>
+      </c>
+      <c r="F65" t="n">
+        <v>26</v>
+      </c>
+      <c r="G65" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B66" t="n">
+        <v>25</v>
+      </c>
+      <c r="C66" t="n">
+        <v>27</v>
+      </c>
+      <c r="D66" t="n">
+        <v>27</v>
+      </c>
+      <c r="E66" t="n">
+        <v>26</v>
+      </c>
+      <c r="F66" t="n">
+        <v>26</v>
+      </c>
+      <c r="G66" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B67" t="n">
+        <v>24</v>
+      </c>
+      <c r="C67" t="n">
+        <v>27</v>
+      </c>
+      <c r="D67" t="n">
+        <v>27</v>
+      </c>
+      <c r="E67" t="n">
+        <v>24</v>
+      </c>
+      <c r="F67" t="n">
+        <v>27</v>
+      </c>
+      <c r="G67" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B68" t="n">
+        <v>26</v>
+      </c>
+      <c r="C68" t="n">
+        <v>27</v>
+      </c>
+      <c r="D68" t="n">
+        <v>28</v>
+      </c>
+      <c r="E68" t="n">
+        <v>27</v>
+      </c>
+      <c r="F68" t="n">
+        <v>27</v>
+      </c>
+      <c r="G68" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B69" t="n">
+        <v>26</v>
+      </c>
+      <c r="C69" t="n">
+        <v>28</v>
+      </c>
+      <c r="D69" t="n">
+        <v>28</v>
+      </c>
+      <c r="E69" t="n">
+        <v>27</v>
+      </c>
+      <c r="F69" t="n">
+        <v>28</v>
+      </c>
+      <c r="G69" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B70" t="n">
+        <v>25</v>
+      </c>
+      <c r="C70" t="n">
+        <v>28</v>
+      </c>
+      <c r="D70" t="n">
+        <v>29</v>
+      </c>
+      <c r="E70" t="n">
+        <v>25</v>
+      </c>
+      <c r="F70" t="n">
+        <v>27</v>
+      </c>
+      <c r="G70" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B71" t="n">
+        <v>27</v>
+      </c>
+      <c r="C71" t="n">
+        <v>29</v>
+      </c>
+      <c r="D71" t="n">
+        <v>29</v>
+      </c>
+      <c r="E71" t="n">
+        <v>28</v>
+      </c>
+      <c r="F71" t="n">
+        <v>29</v>
+      </c>
+      <c r="G71" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B72" t="n">
+        <v>27</v>
+      </c>
+      <c r="C72" t="n">
+        <v>28</v>
+      </c>
+      <c r="D72" t="n">
+        <v>29</v>
+      </c>
+      <c r="E72" t="n">
+        <v>28</v>
+      </c>
+      <c r="F72" t="n">
+        <v>29</v>
+      </c>
+      <c r="G72" t="n">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
n od 7 do 80
</commit_message>
<xml_diff>
--- a/rezultati_naloga_2.xlsx
+++ b/rezultati_naloga_2.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1012,6 +1012,30 @@
         <v>31</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B73" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B74" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B75" t="n">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1023,7 +1047,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2669,6 +2693,75 @@
         <v>28</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B73" t="n">
+        <v>26</v>
+      </c>
+      <c r="C73" t="n">
+        <v>30</v>
+      </c>
+      <c r="D73" t="n">
+        <v>30</v>
+      </c>
+      <c r="E73" t="n">
+        <v>26</v>
+      </c>
+      <c r="F73" t="n">
+        <v>28</v>
+      </c>
+      <c r="G73" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B74" t="n">
+        <v>28</v>
+      </c>
+      <c r="C74" t="n">
+        <v>30</v>
+      </c>
+      <c r="D74" t="n">
+        <v>30</v>
+      </c>
+      <c r="E74" t="n">
+        <v>29</v>
+      </c>
+      <c r="F74" t="n">
+        <v>30</v>
+      </c>
+      <c r="G74" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B75" t="n">
+        <v>28</v>
+      </c>
+      <c r="C75" t="n">
+        <v>30</v>
+      </c>
+      <c r="D75" t="n">
+        <v>30</v>
+      </c>
+      <c r="E75" t="n">
+        <v>29</v>
+      </c>
+      <c r="F75" t="n">
+        <v>30</v>
+      </c>
+      <c r="G75" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>